<commit_message>
added some prony optimisation functionality
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -67,12 +67,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,156 +361,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>4.5999999999999999E-3</v>
+        <v>4.3852522981429898</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1">
-        <v>20.607299999999999</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.91812208017774677</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>0.96150000000000002</v>
+        <v>1999.1997237981018</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9344887962828148</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>3.32E-2</v>
+        <v>1999.9109564015557</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1662.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>4.5999999999999999E-3</v>
+        <v>4.3852522981429898</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>20.607299999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>0.96150000000000002</v>
+        <v>1948.8112191007419</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>3.32E-2</v>
+        <v>1999.9109564015557</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1662.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
-        <v>4.5999999999999999E-3</v>
+        <v>4.3852522981429898</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>20.607299999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0000028307354387</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>0.96150000000000002</v>
+        <v>1999.1997237981018</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.0582701916491977</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>3.32E-2</v>
+        <v>1966.4713886262534</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1662.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10">
-        <v>4.5999999999999999E-3</v>
+        <v>4.1097887301611271</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>20.607299999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>0.96150000000000002</v>
+        <v>1948.8112191007419</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>3.32E-2</v>
+        <v>1999.9109564015557</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1662.1</v>
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13">
+        <v>4.1337651205162977</v>
+      </c>
+      <c r="D13">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D14">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D15">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D16">
+        <v>0.91363282242797661</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D17">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18">
+        <v>1956.695694839528</v>
+      </c>
+      <c r="D18">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D19">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D20">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D21">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D22">
+        <v>0.92284345562515302</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D23">
+        <v>1.9944153329789898</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24">
+        <v>2026.3291249280892</v>
+      </c>
+      <c r="D24">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D25">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D26">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D27">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D28">
+        <v>0.91812208017774677</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D29">
+        <v>1.9344887962828148</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D30">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D31">
+        <v>0.92284345562515302</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D32">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33">
+        <v>2026.3291249280892</v>
+      </c>
+      <c r="D33">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D34">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D35">
+        <v>1.9944153329789898</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D36">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D37">
+        <v>0.92284345562515302</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38">
+        <v>1999.3038323636138</v>
+      </c>
+      <c r="D38">
+        <v>1.9944153329789898</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39">
+        <v>2026.3291249280892</v>
+      </c>
+      <c r="D39">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D40">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D41">
+        <v>4.6117341589867173</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D42">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43">
+        <v>4.5579809086431569</v>
+      </c>
+      <c r="D43">
+        <v>1.0000028307354387</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44">
+        <v>1999.4900873532908</v>
+      </c>
+      <c r="D44">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D45">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D46">
+        <v>0.92284345562515302</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D47">
+        <v>1.9944153329789898</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48">
+        <v>2026.4418055131312</v>
+      </c>
+      <c r="D48">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49">
+        <v>4.1337651205162977</v>
+      </c>
+      <c r="D49">
+        <v>0.91363282242797661</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D50">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51">
+        <v>1956.695694839528</v>
+      </c>
+      <c r="D51">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52">
+        <v>4.1337651205162977</v>
+      </c>
+      <c r="D52">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53">
+        <v>1999.2844452333702</v>
+      </c>
+      <c r="D53">
+        <v>18.019977517561315</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54">
+        <v>1956.695694839528</v>
+      </c>
+      <c r="D54">
+        <v>33.476097728275242</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55">
+        <v>4.1337651205162977</v>
+      </c>
+      <c r="D55">
+        <v>4.8173538419420172</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D56">
+        <v>7.0059410099920782</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57">
+        <v>1956.543242198072</v>
+      </c>
+      <c r="D57">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58">
+        <v>4.2404515431641761</v>
+      </c>
+      <c r="D58">
+        <v>0.9331223291568056</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59">
+        <v>1948.8112191007419</v>
+      </c>
+      <c r="D59">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60">
+        <v>1999.8272574423142</v>
+      </c>
+      <c r="D60">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61">
+        <v>4.3852522981429898</v>
+      </c>
+      <c r="D61">
+        <v>0.91812208017774677</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D62">
+        <v>1.9344887962828148</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63">
+        <v>2000.0654368712253</v>
+      </c>
+      <c r="D63">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64">
+        <v>4.5579809086431569</v>
+      </c>
+      <c r="D64">
+        <v>1.0000028307354387</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D65">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66">
+        <v>1999.9109564015557</v>
+      </c>
+      <c r="D66">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67">
+        <v>4.1097887301611271</v>
+      </c>
+      <c r="D67">
+        <v>1.0000028307354387</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D68">
+        <v>2.0582701916491977</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69">
+        <v>1966.2607593986083</v>
+      </c>
+      <c r="D69">
+        <v>18.000801368082428</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70">
+        <v>4.1337651205162977</v>
+      </c>
+      <c r="D70">
+        <v>0.91363282242797661</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71">
+        <v>1999.1997237981018</v>
+      </c>
+      <c r="D71">
+        <v>2.0008015903931873</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72">
+        <v>1956.695694839528</v>
+      </c>
+      <c r="D72">
+        <v>18.000801368082428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the progrmam to run for only 1 seconbd during the viscoelastic portion of the test to match experimental output, to aid in validation of the models.
added in the validation data set that currently only includes the ramp portion of the data
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -90,11 +90,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D30"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="true"/>
-    <col min="2" max="2" width="13.7109375" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
     <col min="3" max="3" width="2.140625" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
   </cols>
@@ -104,7 +104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>0.041459996931306073</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C1" s="0">
         <v>0</v>
@@ -116,73 +116,71 @@
     <row r="2">
       <c r="A2" s="0"/>
       <c r="B2" s="0">
-        <v>0.95845173064227707</v>
+        <v>0.33097849740403568</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="A3" s="0"/>
       <c r="B3" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.63966597399175562</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>1</v>
+        <v>1.0009289780615449</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0"/>
+      <c r="A4" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="B4" s="0">
-        <v>0.87039998284470466</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C4" s="0">
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>1.0007404164892799</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="0"/>
       <c r="B5" s="0">
-        <v>0.041459996931306073</v>
+        <v>0.4581262659541554</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>1</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0"/>
       <c r="B6" s="0">
-        <v>0.95845173064227707</v>
+        <v>0.43649209069039513</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.001653698601076</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.032359718601307222</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
@@ -194,73 +192,71 @@
     <row r="8">
       <c r="A8" s="0"/>
       <c r="B8" s="0">
-        <v>0.77293928445731019</v>
+        <v>0.69768280919871917</v>
       </c>
       <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="A9" s="0"/>
       <c r="B9" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.26995747219997357</v>
       </c>
       <c r="C9" s="0">
         <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>1</v>
+        <v>1.001653698601076</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0"/>
+      <c r="A10" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="B10" s="0">
-        <v>0.71431833235231401</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C10" s="0">
         <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>1.0007404164892799</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="A11" s="0"/>
       <c r="B11" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.28504821933620944</v>
       </c>
       <c r="C11" s="0">
         <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>1</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0"/>
       <c r="B12" s="0">
-        <v>0.56573545209779064</v>
+        <v>0.63966597399175562</v>
       </c>
       <c r="C12" s="0">
         <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.001653698601076</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C13" s="0">
         <v>0</v>
@@ -272,73 +268,71 @@
     <row r="14">
       <c r="A14" s="0"/>
       <c r="B14" s="0">
-        <v>0.48021596554089035</v>
+        <v>0.24935449218334294</v>
       </c>
       <c r="C14" s="0">
         <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A15" s="0"/>
       <c r="B15" s="0">
-        <v>0.092599224070642111</v>
+        <v>0.69100741699239687</v>
       </c>
       <c r="C15" s="0">
         <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>1</v>
+        <v>1.001653698601076</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0"/>
+      <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="B16" s="0">
-        <v>0.90740077592935797</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C16" s="0">
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>1.0007404164892799</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A17" s="0"/>
       <c r="B17" s="0">
-        <v>0.041459996931306073</v>
+        <v>0.33097849740403568</v>
       </c>
       <c r="C17" s="0">
         <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>1</v>
+        <v>1.0000000100443873</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0"/>
       <c r="B18" s="0">
-        <v>0.95845173064227707</v>
+        <v>0.49232107515928952</v>
       </c>
       <c r="C18" s="0">
         <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.001653698601076</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" s="0">
-        <v>0.041036291232258201</v>
+        <v>0.029355528604208678</v>
       </c>
       <c r="C19" s="0">
         <v>0</v>
@@ -350,13 +344,139 @@
     <row r="20">
       <c r="A20" s="0"/>
       <c r="B20" s="0">
-        <v>0.87687375166927328</v>
+        <v>0.33097849740403568</v>
       </c>
       <c r="C20" s="0">
         <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>1.0007404164892799</v>
+        <v>1.0000000100443873</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0">
+        <v>0.44100978663522117</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0">
+        <v>1.001653698601076</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.029355528604208678</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0"/>
+      <c r="B23" s="0">
+        <v>0.3905073882079626</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0">
+        <v>1.0000000100443873</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0">
+        <v>0.3716967101964278</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0">
+        <v>1.001653698601076</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0.029355528604208678</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0">
+        <v>0.20309524364030435</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0">
+        <v>1.0000000100443873</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0">
+        <v>0.75904029968273135</v>
+      </c>
+      <c r="C27" s="0">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0">
+        <v>1.001653698601076</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.029355528604208678</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0">
+        <v>0.22104725323730129</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0">
+        <v>1.0000000100443873</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0">
+        <v>0.63966597399175562</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0">
+        <v>1.001653698601076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed an issue where it wouldnt run if N = 1.
Algorithm fixed now.
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -90,11 +90,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D50"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="true"/>
-    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true"/>
     <col min="3" max="3" width="2.140625" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
   </cols>
@@ -104,7 +104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.034147898981497074</v>
       </c>
       <c r="C1" s="0">
         <v>0</v>
@@ -116,185 +116,181 @@
     <row r="2">
       <c r="A2" s="0"/>
       <c r="B2" s="0">
-        <v>0.33097849740403568</v>
+        <v>0.033436865941310283</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0000000242688842</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0"/>
       <c r="B3" s="0">
-        <v>0.63966597399175562</v>
+        <v>0.30886321085420804</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>1.0009289780615449</v>
+        <v>1.0002508772307033</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="A4" s="0"/>
       <c r="B4" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.31230550096784959</v>
       </c>
       <c r="C4" s="0">
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>1</v>
+        <v>1.0018701191037918</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0"/>
       <c r="B5" s="0">
-        <v>0.4581262659541554</v>
+        <v>0.31124652325513502</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0"/>
+      <c r="A6" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="B6" s="0">
-        <v>0.43649209069039513</v>
+        <v>0.030722527803756637</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>1.001653698601076</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="0"/>
       <c r="B7" s="0">
-        <v>0.032359718601307222</v>
+        <v>0.030082818392692584</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>1</v>
+        <v>1.0000000242688842</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0"/>
       <c r="B8" s="0">
-        <v>0.69768280919871917</v>
+        <v>0.27788118350026658</v>
       </c>
       <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0005739071473685</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0"/>
       <c r="B9" s="0">
-        <v>0.26995747219997357</v>
+        <v>0.38128804415013301</v>
       </c>
       <c r="C9" s="0">
         <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="0"/>
       <c r="B10" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.28002542615315112</v>
       </c>
       <c r="C10" s="0">
         <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>1</v>
+        <v>1.0040163366135519</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0"/>
+      <c r="A11" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="B11" s="0">
-        <v>0.28504821933620944</v>
+        <v>0.23640719556630729</v>
       </c>
       <c r="C11" s="0">
         <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>1.0000000100443873</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0"/>
       <c r="B12" s="0">
-        <v>0.63966597399175562</v>
+        <v>0.026434844639955303</v>
       </c>
       <c r="C12" s="0">
         <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0004015525554197</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="0"/>
       <c r="B13" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.24418409931899246</v>
       </c>
       <c r="C13" s="0">
         <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>1</v>
+        <v>1.0005739071473685</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0"/>
       <c r="B14" s="0">
-        <v>0.24935449218334294</v>
+        <v>0.24690553871823187</v>
       </c>
       <c r="C14" s="0">
         <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0018701191037918</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0"/>
       <c r="B15" s="0">
-        <v>0.69100741699239687</v>
+        <v>0.246068321756513</v>
       </c>
       <c r="C15" s="0">
         <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.034147898666879346</v>
       </c>
       <c r="C16" s="0">
         <v>0</v>
@@ -306,177 +302,421 @@
     <row r="17">
       <c r="A17" s="0"/>
       <c r="B17" s="0">
-        <v>0.33097849740403568</v>
+        <v>0.033436874846628148</v>
       </c>
       <c r="C17" s="0">
         <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0000000242688842</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0"/>
       <c r="B18" s="0">
-        <v>0.49232107515928952</v>
+        <v>0.35766313583148418</v>
       </c>
       <c r="C18" s="0">
         <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0005739071473685</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0" t="s">
-        <v>6</v>
-      </c>
+      <c r="A19" s="0"/>
       <c r="B19" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.24950642694818248</v>
       </c>
       <c r="C19" s="0">
         <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>1</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0"/>
       <c r="B20" s="0">
-        <v>0.33097849740403568</v>
+        <v>0.31124652038750111</v>
       </c>
       <c r="C20" s="0">
         <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0040163366135519</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0"/>
+      <c r="A21" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="B21" s="0">
-        <v>0.44100978663522117</v>
+        <v>0.028008528417434175</v>
       </c>
       <c r="C21" s="0">
         <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>1.001653698601076</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A22" s="0"/>
       <c r="B22" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.20721298191153933</v>
       </c>
       <c r="C22" s="0">
         <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>1</v>
+        <v>1.0004015525554197</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0"/>
       <c r="B23" s="0">
-        <v>0.3905073882079626</v>
+        <v>0.25333341951718491</v>
       </c>
       <c r="C23" s="0">
         <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0005739071473685</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0"/>
       <c r="B24" s="0">
-        <v>0.3716967101964278</v>
+        <v>0.2561568283752591</v>
       </c>
       <c r="C24" s="0">
         <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0018701191037918</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A25" s="0"/>
       <c r="B25" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.2552882417785825</v>
       </c>
       <c r="C25" s="0">
         <v>0</v>
       </c>
       <c r="D25" s="0">
-        <v>1</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0"/>
+      <c r="A26" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="B26" s="0">
-        <v>0.20309524364030435</v>
+        <v>0.034147898981497074</v>
       </c>
       <c r="C26" s="0">
         <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>1.0000000100443873</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0"/>
       <c r="B27" s="0">
-        <v>0.75904029968273135</v>
+        <v>0.033436865941310283</v>
       </c>
       <c r="C27" s="0">
         <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0000000242688842</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A28" s="0"/>
       <c r="B28" s="0">
-        <v>0.029355528604208678</v>
+        <v>0.30886321085420804</v>
       </c>
       <c r="C28" s="0">
         <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>1</v>
+        <v>1.0002508772307033</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0"/>
       <c r="B29" s="0">
-        <v>0.22104725323730129</v>
+        <v>0.35171567389996311</v>
       </c>
       <c r="C29" s="0">
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>1.0000000100443873</v>
+        <v>1.0023366633433919</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0"/>
       <c r="B30" s="0">
-        <v>0.63966597399175562</v>
+        <v>0.24612987588780932</v>
       </c>
       <c r="C30" s="0">
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>1.001653698601076</v>
+        <v>1.0040163366135519</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0.18633904568355625</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0">
+        <v>0.028168155582483253</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0">
+        <v>1.0000000242688842</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0">
+        <v>0.2601950491507618</v>
+      </c>
+      <c r="C33" s="0">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0">
+        <v>1.0005739071473685</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0">
+        <v>0.26309493108501042</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0">
+        <v>1.0023366633433919</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0">
+        <v>0.26220281849818833</v>
+      </c>
+      <c r="C35" s="0">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0">
+        <v>1.0040163366135519</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="0">
+        <v>0.034147898981497074</v>
+      </c>
+      <c r="C36" s="0">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0">
+        <v>0.033436865941310283</v>
+      </c>
+      <c r="C37" s="0">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0">
+        <v>1.0000000242688842</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0">
+        <v>0.45274024457639483</v>
+      </c>
+      <c r="C38" s="0">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0">
+        <v>1.0002508772307033</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0">
+        <v>0.24014510273020398</v>
+      </c>
+      <c r="C39" s="0">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1.0023366633433919</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0">
+        <v>0.23933080931935874</v>
+      </c>
+      <c r="C40" s="0">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0">
+        <v>1.0040163366135519</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0.034147898981497074</v>
+      </c>
+      <c r="C41" s="0">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0">
+        <v>0.033436865941310283</v>
+      </c>
+      <c r="C42" s="0">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0">
+        <v>1.0000000242688842</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0">
+        <v>0.39094647271240951</v>
+      </c>
+      <c r="C43" s="0">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0">
+        <v>1.0002508772307033</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0">
+        <v>0.31230550096784959</v>
+      </c>
+      <c r="C44" s="0">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0">
+        <v>1.0023366633433919</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0">
+        <v>0.21342248879097966</v>
+      </c>
+      <c r="C45" s="0">
+        <v>0</v>
+      </c>
+      <c r="D45" s="0">
+        <v>1.0040163366135519</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0.028674084599537873</v>
+      </c>
+      <c r="C46" s="0">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0">
+        <v>0.028077028202058488</v>
+      </c>
+      <c r="C47" s="0">
+        <v>0</v>
+      </c>
+      <c r="D47" s="0">
+        <v>1.0004015525554197</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0"/>
+      <c r="B48" s="0">
+        <v>0.25935328678690484</v>
+      </c>
+      <c r="C48" s="0">
+        <v>0</v>
+      </c>
+      <c r="D48" s="0">
+        <v>1.0005739071473685</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0">
+        <v>0.26224378725336672</v>
+      </c>
+      <c r="C49" s="0">
+        <v>0</v>
+      </c>
+      <c r="D49" s="0">
+        <v>1.0018701191037918</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0">
+        <v>0.42165181315813205</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0">
+        <v>1.0023366633433919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a number of additions and changes to code base
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D40"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="true"/>
@@ -104,7 +104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>0.034147898981497074</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C1" s="0">
         <v>0</v>
@@ -116,243 +116,245 @@
     <row r="2">
       <c r="A2" s="0"/>
       <c r="B2" s="0">
-        <v>0.033436865941310283</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>1.0000000242688842</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0"/>
       <c r="B3" s="0">
-        <v>0.30886321085420804</v>
+        <v>0.10038393564714866</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>1.0002508772307033</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0"/>
       <c r="B4" s="0">
-        <v>0.31230550096784959</v>
+        <v>0.83227844973102871</v>
       </c>
       <c r="C4" s="0">
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>1.0018701191037918</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0"/>
+      <c r="A5" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="B5" s="0">
-        <v>0.31124652325513502</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>1.0023366633433919</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="A6" s="0"/>
       <c r="B6" s="0">
-        <v>0.030722527803756637</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>1</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0"/>
       <c r="B7" s="0">
-        <v>0.030082818392692584</v>
+        <v>0.10038393564714866</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>1.0000000242688842</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0"/>
       <c r="B8" s="0">
-        <v>0.27788118350026658</v>
+        <v>0.76440718752323167</v>
       </c>
       <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>1.0005739071473685</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0"/>
+      <c r="A9" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="B9" s="0">
-        <v>0.38128804415013301</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C9" s="0">
         <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>1.0023366633433919</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0"/>
       <c r="B10" s="0">
-        <v>0.28002542615315112</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C10" s="0">
         <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>1.0040163366135519</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="A11" s="0"/>
       <c r="B11" s="0">
-        <v>0.23640719556630729</v>
+        <v>0.14156624958095382</v>
       </c>
       <c r="C11" s="0">
         <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>1</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0"/>
       <c r="B12" s="0">
-        <v>0.026434844639955303</v>
+        <v>0.75941879239032173</v>
       </c>
       <c r="C12" s="0">
         <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>1.0004015525554197</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0"/>
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="B13" s="0">
-        <v>0.24418409931899246</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C13" s="0">
         <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>1.0005739071473685</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0"/>
       <c r="B14" s="0">
-        <v>0.24690553871823187</v>
+        <v>0.10469062282257531</v>
       </c>
       <c r="C14" s="0">
         <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>1.0018701191037918</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0"/>
       <c r="B15" s="0">
-        <v>0.246068321756513</v>
+        <v>0.045281251729978669</v>
       </c>
       <c r="C15" s="0">
         <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>1.0023366633433919</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16" s="0"/>
       <c r="B16" s="0">
-        <v>0.034147898666879346</v>
+        <v>0.6337512757736149</v>
       </c>
       <c r="C16" s="0">
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>1</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0"/>
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" s="0">
-        <v>0.033436874846628148</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C17" s="0">
         <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>1.0000000242688842</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0"/>
       <c r="B18" s="0">
-        <v>0.35766313583148418</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C18" s="0">
         <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>1.0005739071473685</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0"/>
       <c r="B19" s="0">
-        <v>0.24950642694818248</v>
+        <v>0.10038393564714866</v>
       </c>
       <c r="C19" s="0">
         <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>1.0023366633433919</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0"/>
       <c r="B20" s="0">
-        <v>0.31124652038750111</v>
+        <v>0.54639166289359131</v>
       </c>
       <c r="C20" s="0">
         <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>1.0040163366135519</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="0">
-        <v>0.028008528417434175</v>
+        <v>0.11306720158455907</v>
       </c>
       <c r="C21" s="0">
         <v>0</v>
@@ -364,359 +366,237 @@
     <row r="22">
       <c r="A22" s="0"/>
       <c r="B22" s="0">
-        <v>0.20721298191153933</v>
+        <v>0.048092939096244326</v>
       </c>
       <c r="C22" s="0">
         <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>1.0004015525554197</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0"/>
       <c r="B23" s="0">
-        <v>0.25333341951718491</v>
+        <v>0.10038393564714866</v>
       </c>
       <c r="C23" s="0">
         <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>1.0005739071473685</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0"/>
       <c r="B24" s="0">
-        <v>0.2561568283752591</v>
+        <v>0.71133576772740081</v>
       </c>
       <c r="C24" s="0">
         <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>1.0018701191037918</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0"/>
+      <c r="A25" s="0" t="s">
+        <v>6</v>
+      </c>
       <c r="B25" s="0">
-        <v>0.2552882417785825</v>
+        <v>0.077336063449010645</v>
       </c>
       <c r="C25" s="0">
         <v>0</v>
       </c>
       <c r="D25" s="0">
-        <v>1.0023366633433919</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="A26" s="0"/>
       <c r="B26" s="0">
-        <v>0.034147898981497074</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C26" s="0">
         <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>1</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0"/>
       <c r="B27" s="0">
-        <v>0.033436865941310283</v>
+        <v>0.10038393564714866</v>
       </c>
       <c r="C27" s="0">
         <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>1.0000000242688842</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0"/>
       <c r="B28" s="0">
-        <v>0.30886321085420804</v>
+        <v>0.57692608537559342</v>
       </c>
       <c r="C28" s="0">
         <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>1.0002508772307033</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="0"/>
+      <c r="A29" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="B29" s="0">
-        <v>0.35171567389996311</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C29" s="0">
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>1.0023366633433919</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0"/>
       <c r="B30" s="0">
-        <v>0.24612987588780932</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C30" s="0">
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>1.0040163366135519</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="0" t="s">
-        <v>6</v>
-      </c>
+      <c r="A31" s="0"/>
       <c r="B31" s="0">
-        <v>0.18633904568355625</v>
+        <v>0.15030093508922987</v>
       </c>
       <c r="C31" s="0">
         <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>1</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0"/>
       <c r="B32" s="0">
-        <v>0.028168155582483253</v>
+        <v>0.46470267772662122</v>
       </c>
       <c r="C32" s="0">
         <v>0</v>
       </c>
       <c r="D32" s="0">
-        <v>1.0000000242688842</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="0"/>
+      <c r="A33" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B33" s="0">
-        <v>0.2601950491507618</v>
+        <v>0.033066361824819576</v>
       </c>
       <c r="C33" s="0">
         <v>0</v>
       </c>
       <c r="D33" s="0">
-        <v>1.0005739071473685</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0"/>
       <c r="B34" s="0">
-        <v>0.26309493108501042</v>
+        <v>0.0342711652944198</v>
       </c>
       <c r="C34" s="0">
         <v>0</v>
       </c>
       <c r="D34" s="0">
-        <v>1.0023366633433919</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0"/>
       <c r="B35" s="0">
-        <v>0.26220281849818833</v>
+        <v>0.23695651644201202</v>
       </c>
       <c r="C35" s="0">
         <v>0</v>
       </c>
       <c r="D35" s="0">
-        <v>1.0040163366135519</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A36" s="0"/>
       <c r="B36" s="0">
-        <v>0.034147898981497074</v>
+        <v>0.46985792404686311</v>
       </c>
       <c r="C36" s="0">
         <v>0</v>
       </c>
       <c r="D36" s="0">
-        <v>1</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="0"/>
+      <c r="A37" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="B37" s="0">
-        <v>0.033436865941310283</v>
+        <v>0.021741871350707601</v>
       </c>
       <c r="C37" s="0">
         <v>0</v>
       </c>
       <c r="D37" s="0">
-        <v>1.0000000242688842</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0"/>
       <c r="B38" s="0">
-        <v>0.45274024457639483</v>
+        <v>0.07016406560419558</v>
       </c>
       <c r="C38" s="0">
         <v>0</v>
       </c>
       <c r="D38" s="0">
-        <v>1.0002508772307033</v>
+        <v>2.0000001078564171</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0"/>
       <c r="B39" s="0">
-        <v>0.24014510273020398</v>
+        <v>0.038862458442287973</v>
       </c>
       <c r="C39" s="0">
         <v>0</v>
       </c>
       <c r="D39" s="0">
-        <v>1.0023366633433919</v>
+        <v>4.0000003330430003</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0"/>
       <c r="B40" s="0">
-        <v>0.23933080931935874</v>
+        <v>0.83227844973102871</v>
       </c>
       <c r="C40" s="0">
         <v>0</v>
       </c>
       <c r="D40" s="0">
-        <v>1.0040163366135519</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="0">
-        <v>0.034147898981497074</v>
-      </c>
-      <c r="C41" s="0">
-        <v>0</v>
-      </c>
-      <c r="D41" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0">
-        <v>0.033436865941310283</v>
-      </c>
-      <c r="C42" s="0">
-        <v>0</v>
-      </c>
-      <c r="D42" s="0">
-        <v>1.0000000242688842</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0">
-        <v>0.39094647271240951</v>
-      </c>
-      <c r="C43" s="0">
-        <v>0</v>
-      </c>
-      <c r="D43" s="0">
-        <v>1.0002508772307033</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0">
-        <v>0.31230550096784959</v>
-      </c>
-      <c r="C44" s="0">
-        <v>0</v>
-      </c>
-      <c r="D44" s="0">
-        <v>1.0023366633433919</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="0"/>
-      <c r="B45" s="0">
-        <v>0.21342248879097966</v>
-      </c>
-      <c r="C45" s="0">
-        <v>0</v>
-      </c>
-      <c r="D45" s="0">
-        <v>1.0040163366135519</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="0">
-        <v>0.028674084599537873</v>
-      </c>
-      <c r="C46" s="0">
-        <v>0</v>
-      </c>
-      <c r="D46" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="0"/>
-      <c r="B47" s="0">
-        <v>0.028077028202058488</v>
-      </c>
-      <c r="C47" s="0">
-        <v>0</v>
-      </c>
-      <c r="D47" s="0">
-        <v>1.0004015525554197</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="0"/>
-      <c r="B48" s="0">
-        <v>0.25935328678690484</v>
-      </c>
-      <c r="C48" s="0">
-        <v>0</v>
-      </c>
-      <c r="D48" s="0">
-        <v>1.0005739071473685</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="0"/>
-      <c r="B49" s="0">
-        <v>0.26224378725336672</v>
-      </c>
-      <c r="C49" s="0">
-        <v>0</v>
-      </c>
-      <c r="D49" s="0">
-        <v>1.0018701191037918</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="0"/>
-      <c r="B50" s="0">
-        <v>0.42165181315813205</v>
-      </c>
-      <c r="C50" s="0">
-        <v>0</v>
-      </c>
-      <c r="D50" s="0">
-        <v>1.0023366633433919</v>
+        <v>8.0000009394871583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A number of changes -added extra parameter retrieval in python scripts -fixed organisation of results from model runs -established validation data set
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D30"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="true"/>
@@ -104,7 +104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.10492737431191633</v>
       </c>
       <c r="C1" s="0">
         <v>0</v>
@@ -116,145 +116,147 @@
     <row r="2">
       <c r="A2" s="0"/>
       <c r="B2" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>2.0000001078564171</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0"/>
       <c r="B3" s="0">
-        <v>0.10038393564714866</v>
+        <v>0.85613252551884944</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>4.0000003330430003</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0"/>
+      <c r="A4" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="B4" s="0">
-        <v>0.83227844973102871</v>
+        <v>0.10492737431191633</v>
       </c>
       <c r="C4" s="0">
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>8.0000009394871583</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="A5" s="0"/>
       <c r="B5" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>1</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0"/>
       <c r="B6" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.75854750988127484</v>
       </c>
       <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>2.0000001078564171</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0"/>
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="B7" s="0">
-        <v>0.10038393564714866</v>
+        <v>0.033366215635962093</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>4.0000003330430003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0"/>
       <c r="B8" s="0">
-        <v>0.76440718752323167</v>
+        <v>0.097905244727746435</v>
       </c>
       <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>8.0000009394871583</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>2</v>
-      </c>
+      <c r="A9" s="0"/>
       <c r="B9" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.85613252551884944</v>
       </c>
       <c r="C9" s="0">
         <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>1</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0"/>
+      <c r="A10" s="0" t="s">
+        <v>3</v>
+      </c>
       <c r="B10" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.10492737431191633</v>
       </c>
       <c r="C10" s="0">
         <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>2.0000001078564171</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0"/>
       <c r="B11" s="0">
-        <v>0.14156624958095382</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C11" s="0">
         <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>4.0000003330430003</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0"/>
       <c r="B12" s="0">
-        <v>0.75941879239032173</v>
+        <v>0.68526406177351395</v>
       </c>
       <c r="C12" s="0">
         <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>8.0000009394871583</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.16019338760293667</v>
       </c>
       <c r="C13" s="0">
         <v>0</v>
@@ -266,145 +268,147 @@
     <row r="14">
       <c r="A14" s="0"/>
       <c r="B14" s="0">
-        <v>0.10469062282257531</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C14" s="0">
         <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>2.0000001078564171</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0"/>
       <c r="B15" s="0">
-        <v>0.045281251729978669</v>
+        <v>0.64309330896124162</v>
       </c>
       <c r="C15" s="0">
         <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>4.0000003330430003</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0"/>
+      <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="B16" s="0">
-        <v>0.6337512757736149</v>
+        <v>0.15400444470042224</v>
       </c>
       <c r="C16" s="0">
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>8.0000009394871583</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="A17" s="0"/>
       <c r="B17" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C17" s="0">
         <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>1</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0"/>
       <c r="B18" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.57785008159043016</v>
       </c>
       <c r="C18" s="0">
         <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>2.0000001078564171</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0"/>
+      <c r="A19" s="0" t="s">
+        <v>6</v>
+      </c>
       <c r="B19" s="0">
-        <v>0.10038393564714866</v>
+        <v>0.10492737431191633</v>
       </c>
       <c r="C19" s="0">
         <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>4.0000003330430003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0"/>
       <c r="B20" s="0">
-        <v>0.54639166289359131</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C20" s="0">
         <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>8.0000009394871583</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="A21" s="0"/>
       <c r="B21" s="0">
-        <v>0.11306720158455907</v>
+        <v>0.63611864135280316</v>
       </c>
       <c r="C21" s="0">
         <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>1</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0"/>
+      <c r="A22" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="B22" s="0">
-        <v>0.048092939096244326</v>
+        <v>0.10492737431191633</v>
       </c>
       <c r="C22" s="0">
         <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>2.0000001078564171</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0"/>
       <c r="B23" s="0">
-        <v>0.10038393564714866</v>
+        <v>0.028636878962368204</v>
       </c>
       <c r="C23" s="0">
         <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>4.0000003330430003</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0"/>
       <c r="B24" s="0">
-        <v>0.71133576772740081</v>
+        <v>0.56455453080286322</v>
       </c>
       <c r="C24" s="0">
         <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>8.0000009394871583</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25" s="0">
-        <v>0.077336063449010645</v>
+        <v>0.23765155675061522</v>
       </c>
       <c r="C25" s="0">
         <v>0</v>
@@ -416,187 +420,63 @@
     <row r="26">
       <c r="A26" s="0"/>
       <c r="B26" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C26" s="0">
         <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>2.0000001078564171</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0"/>
       <c r="B27" s="0">
-        <v>0.10038393564714866</v>
+        <v>0.39789029008409094</v>
       </c>
       <c r="C27" s="0">
         <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>4.0000003330430003</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="0"/>
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="B28" s="0">
-        <v>0.57692608537559342</v>
+        <v>0.061102364881295543</v>
       </c>
       <c r="C28" s="0">
         <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>8.0000009394871583</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A29" s="0"/>
       <c r="B29" s="0">
-        <v>0.033066361824819576</v>
+        <v>0.038940084023250041</v>
       </c>
       <c r="C29" s="0">
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>1</v>
+        <v>2.0000000095576573</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0"/>
       <c r="B30" s="0">
-        <v>0.0342711652944198</v>
+        <v>0.55809815727170164</v>
       </c>
       <c r="C30" s="0">
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>2.0000001078564171</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0">
-        <v>0.15030093508922987</v>
-      </c>
-      <c r="C31" s="0">
-        <v>0</v>
-      </c>
-      <c r="D31" s="0">
-        <v>4.0000003330430003</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0">
-        <v>0.46470267772662122</v>
-      </c>
-      <c r="C32" s="0">
-        <v>0</v>
-      </c>
-      <c r="D32" s="0">
-        <v>8.0000009394871583</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="0">
-        <v>0.033066361824819576</v>
-      </c>
-      <c r="C33" s="0">
-        <v>0</v>
-      </c>
-      <c r="D33" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0">
-        <v>0.0342711652944198</v>
-      </c>
-      <c r="C34" s="0">
-        <v>0</v>
-      </c>
-      <c r="D34" s="0">
-        <v>2.0000001078564171</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0">
-        <v>0.23695651644201202</v>
-      </c>
-      <c r="C35" s="0">
-        <v>0</v>
-      </c>
-      <c r="D35" s="0">
-        <v>4.0000003330430003</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0">
-        <v>0.46985792404686311</v>
-      </c>
-      <c r="C36" s="0">
-        <v>0</v>
-      </c>
-      <c r="D36" s="0">
-        <v>8.0000009394871583</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="0">
-        <v>0.021741871350707601</v>
-      </c>
-      <c r="C37" s="0">
-        <v>0</v>
-      </c>
-      <c r="D37" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0">
-        <v>0.07016406560419558</v>
-      </c>
-      <c r="C38" s="0">
-        <v>0</v>
-      </c>
-      <c r="D38" s="0">
-        <v>2.0000001078564171</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0">
-        <v>0.038862458442287973</v>
-      </c>
-      <c r="C39" s="0">
-        <v>0</v>
-      </c>
-      <c r="D39" s="0">
-        <v>4.0000003330430003</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0">
-        <v>0.83227844973102871</v>
-      </c>
-      <c r="C40" s="0">
-        <v>0</v>
-      </c>
-      <c r="D40" s="0">
-        <v>8.0000009394871583</v>
+        <v>4.0000000319149764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First complete run of system need to make some changes to data set creation to prioritise the model outputs.
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Visco1</t>
   </si>
@@ -43,6 +43,36 @@
   </si>
   <si>
     <t>Visco10</t>
+  </si>
+  <si>
+    <t>Visco11</t>
+  </si>
+  <si>
+    <t>Visco12</t>
+  </si>
+  <si>
+    <t>Visco13</t>
+  </si>
+  <si>
+    <t>Visco14</t>
+  </si>
+  <si>
+    <t>Visco15</t>
+  </si>
+  <si>
+    <t>Visco16</t>
+  </si>
+  <si>
+    <t>Visco17</t>
+  </si>
+  <si>
+    <t>Visco18</t>
+  </si>
+  <si>
+    <t>Visco19</t>
+  </si>
+  <si>
+    <t>Visco20</t>
   </si>
 </sst>
 </file>
@@ -94,13 +124,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D60"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5859375" customWidth="true"/>
     <col min="2" max="2" width="13.7109375" customWidth="true"/>
     <col min="3" max="3" width="2.2109375" customWidth="true"/>
-    <col min="4" max="4" width="2.2109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -108,7 +138,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.10630000000000001</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -119,7 +149,7 @@
     </row>
     <row r="2">
       <c r="B2">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -130,7 +160,7 @@
     </row>
     <row r="3">
       <c r="B3">
-        <v>0.85465151960280428</v>
+        <v>0.85609999999999997</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -144,7 +174,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.14274244320887408</v>
+        <v>0.14945078156454328</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -155,7 +185,7 @@
     </row>
     <row r="5">
       <c r="B5">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -166,7 +196,7 @@
     </row>
     <row r="6">
       <c r="B6">
-        <v>0.81214949307517126</v>
+        <v>0.78447666500542534</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -180,7 +210,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0.10630000000000001</v>
+        <v>0.16289950236576434</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -191,7 +221,7 @@
     </row>
     <row r="8">
       <c r="B8">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -202,7 +232,7 @@
     </row>
     <row r="9">
       <c r="B9">
-        <v>0.68667247642903773</v>
+        <v>0.64992073947722939</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -216,7 +246,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>0.10630000000000001</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -227,7 +257,7 @@
     </row>
     <row r="11">
       <c r="B11">
-        <v>0.031932311487406016</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -238,7 +268,7 @@
     </row>
     <row r="12">
       <c r="B12">
-        <v>0.73959290834265368</v>
+        <v>0.63980184419543662</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -252,7 +282,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>0.1904505617912732</v>
+        <v>0.051314991585854883</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -263,7 +293,7 @@
     </row>
     <row r="14">
       <c r="B14">
-        <v>0.037900158222271038</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -274,7 +304,7 @@
     </row>
     <row r="15">
       <c r="B15">
-        <v>0.76164927998645582</v>
+        <v>0.90359085899548475</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -288,7 +318,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>0.10630000000000001</v>
+        <v>0.21476120687194955</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -299,7 +329,7 @@
     </row>
     <row r="17">
       <c r="B17">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -310,7 +340,7 @@
     </row>
     <row r="18">
       <c r="B18">
-        <v>0.62312314186800655</v>
+        <v>0.49547994984814642</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -324,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>0.051323633540778679</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -335,7 +365,7 @@
     </row>
     <row r="20">
       <c r="B20">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -346,7 +376,7 @@
     </row>
     <row r="21">
       <c r="B21">
-        <v>0.77077863536545799</v>
+        <v>0.58857854678183441</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -360,7 +390,7 @@
         <v>7</v>
       </c>
       <c r="B22">
-        <v>0.23387354985732539</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -371,7 +401,7 @@
     </row>
     <row r="23">
       <c r="B23">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -382,7 +412,7 @@
     </row>
     <row r="24">
       <c r="B24">
-        <v>0.44265535719745785</v>
+        <v>0.54125110004848132</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -396,7 +426,7 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>0.10630000000000001</v>
+        <v>0.19032199397006488</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -407,7 +437,7 @@
     </row>
     <row r="26">
       <c r="B26">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -418,7 +448,7 @@
     </row>
     <row r="27">
       <c r="B27">
-        <v>0.52177895666050711</v>
+        <v>0.41121321257399401</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -432,7 +462,7 @@
         <v>9</v>
       </c>
       <c r="B28">
-        <v>0.19803897008833632</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -443,7 +473,7 @@
     </row>
     <row r="29">
       <c r="B29">
-        <v>0.038940086068990083</v>
+        <v>0.038899999999999997</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -454,13 +484,373 @@
     </row>
     <row r="30">
       <c r="B30">
-        <v>0.42855373917848499</v>
+        <v>0.46724565895350617</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
         <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>0.025301642045782502</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32">
+        <v>0.038899999999999997</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33">
+        <v>0.62949643765243835</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>0.10001344202317171</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35">
+        <v>0.083648796879183626</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36">
+        <v>0.80633776109764466</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>0.42287438035543634</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38">
+        <v>0.058410056604497954</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39">
+        <v>0.50871556304006582</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>0.12883143677366876</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41">
+        <v>0.038899999999999997</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42">
+        <v>0.36153408907932943</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>0.14004682560972265</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44">
+        <v>0.10244152317586383</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45">
+        <v>0.74751165121441354</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>0.2836237198219313</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47">
+        <v>0.038899999999999997</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48">
+        <v>0.29509858100348535</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>0.095351156470817683</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50">
+        <v>0.12636596457952728</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51">
+        <v>0.76828287894965508</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1.1360228030968871</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53">
+        <v>0.038899999999999997</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>2.2732623201869417</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4.5528301227368324</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55">
+        <v>0.044240679168123381</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56">
+        <v>0.13670771006359447</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57">
+        <v>0.56090523083011179</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59">
+        <v>0.038899999999999997</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2.2319532042837458</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60">
+        <v>0.71097568878688522</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>4.6697648852035627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error with incorrect top solutions being carried through.
</commit_message>
<xml_diff>
--- a/Prony Code/AbacusVariablesVisco.xlsx
+++ b/Prony Code/AbacusVariablesVisco.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Visco1</t>
   </si>
@@ -73,6 +73,96 @@
   </si>
   <si>
     <t>Visco20</t>
+  </si>
+  <si>
+    <t>Visco21</t>
+  </si>
+  <si>
+    <t>Visco22</t>
+  </si>
+  <si>
+    <t>Visco23</t>
+  </si>
+  <si>
+    <t>Visco24</t>
+  </si>
+  <si>
+    <t>Visco25</t>
+  </si>
+  <si>
+    <t>Visco26</t>
+  </si>
+  <si>
+    <t>Visco27</t>
+  </si>
+  <si>
+    <t>Visco28</t>
+  </si>
+  <si>
+    <t>Visco29</t>
+  </si>
+  <si>
+    <t>Visco30</t>
+  </si>
+  <si>
+    <t>Visco31</t>
+  </si>
+  <si>
+    <t>Visco32</t>
+  </si>
+  <si>
+    <t>Visco33</t>
+  </si>
+  <si>
+    <t>Visco34</t>
+  </si>
+  <si>
+    <t>Visco35</t>
+  </si>
+  <si>
+    <t>Visco36</t>
+  </si>
+  <si>
+    <t>Visco37</t>
+  </si>
+  <si>
+    <t>Visco38</t>
+  </si>
+  <si>
+    <t>Visco39</t>
+  </si>
+  <si>
+    <t>Visco40</t>
+  </si>
+  <si>
+    <t>Visco41</t>
+  </si>
+  <si>
+    <t>Visco42</t>
+  </si>
+  <si>
+    <t>Visco43</t>
+  </si>
+  <si>
+    <t>Visco44</t>
+  </si>
+  <si>
+    <t>Visco45</t>
+  </si>
+  <si>
+    <t>Visco46</t>
+  </si>
+  <si>
+    <t>Visco47</t>
+  </si>
+  <si>
+    <t>Visco48</t>
+  </si>
+  <si>
+    <t>Visco49</t>
+  </si>
+  <si>
+    <t>Visco50</t>
   </si>
 </sst>
 </file>
@@ -124,11 +214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D150"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5859375" customWidth="true"/>
-    <col min="2" max="2" width="13.7109375" customWidth="true"/>
+    <col min="2" max="2" width="14.7109375" customWidth="true"/>
     <col min="3" max="3" width="2.2109375" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
   </cols>
@@ -138,7 +228,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.10488490401437629</v>
+        <v>0.14596963032044868</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -149,7 +239,7 @@
     </row>
     <row r="2">
       <c r="B2">
-        <v>0.038899999999999997</v>
+        <v>0.039059735580312727</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -160,7 +250,7 @@
     </row>
     <row r="3">
       <c r="B3">
-        <v>0.85609999999999997</v>
+        <v>0.79081703389162861</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -174,7 +264,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.14945078156454328</v>
+        <v>0.14596963032044868</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -185,7 +275,7 @@
     </row>
     <row r="5">
       <c r="B5">
-        <v>0.038899999999999997</v>
+        <v>0.039059735580312727</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -196,7 +286,7 @@
     </row>
     <row r="6">
       <c r="B6">
-        <v>0.78447666500542534</v>
+        <v>0.79081703389162861</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -210,13 +300,13 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0.16289950236576434</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>1.1360228030968871</v>
       </c>
     </row>
     <row r="8">
@@ -227,18 +317,18 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>2.2732623201869417</v>
       </c>
     </row>
     <row r="9">
       <c r="B9">
-        <v>0.64992073947722939</v>
+        <v>0.85609999999999997</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>4.5528301227368324</v>
       </c>
     </row>
     <row r="10">
@@ -246,7 +336,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>0.10488490401437629</v>
+        <v>0.64842051937131728</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -257,7 +347,7 @@
     </row>
     <row r="11">
       <c r="B11">
-        <v>0.038899999999999997</v>
+        <v>0.17315497379417655</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -268,7 +358,7 @@
     </row>
     <row r="12">
       <c r="B12">
-        <v>0.63980184419543662</v>
+        <v>0.10696446301215579</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -282,7 +372,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>0.051314991585854883</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -293,7 +383,7 @@
     </row>
     <row r="14">
       <c r="B14">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -304,7 +394,7 @@
     </row>
     <row r="15">
       <c r="B15">
-        <v>0.90359085899548475</v>
+        <v>0.77166662098840522</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -318,7 +408,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>0.21476120687194955</v>
+        <v>0.15518016712107413</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -329,7 +419,7 @@
     </row>
     <row r="17">
       <c r="B17">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -340,7 +430,7 @@
     </row>
     <row r="18">
       <c r="B18">
-        <v>0.49547994984814642</v>
+        <v>0.68286915538745374</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -365,7 +455,7 @@
     </row>
     <row r="20">
       <c r="B20">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -376,7 +466,7 @@
     </row>
     <row r="21">
       <c r="B21">
-        <v>0.58857854678183441</v>
+        <v>0.68832078347984738</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -390,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="B22">
-        <v>0.10488490401437629</v>
+        <v>0.16191818565288202</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -401,7 +491,7 @@
     </row>
     <row r="23">
       <c r="B23">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -412,7 +502,7 @@
     </row>
     <row r="24">
       <c r="B24">
-        <v>0.54125110004848132</v>
+        <v>0.59791605318806229</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -426,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>0.19032199397006488</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -437,7 +527,7 @@
     </row>
     <row r="26">
       <c r="B26">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -448,7 +538,7 @@
     </row>
     <row r="27">
       <c r="B27">
-        <v>0.41121321257399401</v>
+        <v>0.58496862906687896</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -462,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="B28">
-        <v>0.10488490401437629</v>
+        <v>0.24497542835466357</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -473,7 +563,7 @@
     </row>
     <row r="29">
       <c r="B29">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -484,7 +574,7 @@
     </row>
     <row r="30">
       <c r="B30">
-        <v>0.46724565895350617</v>
+        <v>0.60007682050648692</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -498,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>0.025301642045782502</v>
+        <v>0.23109011696558016</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -509,7 +599,7 @@
     </row>
     <row r="32">
       <c r="B32">
-        <v>0.038899999999999997</v>
+        <v>0.034104398857726793</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -520,7 +610,7 @@
     </row>
     <row r="33">
       <c r="B33">
-        <v>0.62949643765243835</v>
+        <v>0.7248054841766931</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -534,7 +624,7 @@
         <v>11</v>
       </c>
       <c r="B34">
-        <v>0.10001344202317171</v>
+        <v>0.031255069279608721</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -545,7 +635,7 @@
     </row>
     <row r="35">
       <c r="B35">
-        <v>0.083648796879183626</v>
+        <v>0.16959024592608579</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -556,7 +646,7 @@
     </row>
     <row r="36">
       <c r="B36">
-        <v>0.80633776109764466</v>
+        <v>0.59837877775435999</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -570,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="B37">
-        <v>0.42287438035543634</v>
+        <v>0.15782470034537999</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -581,7 +671,7 @@
     </row>
     <row r="38">
       <c r="B38">
-        <v>0.058410056604497954</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -592,7 +682,7 @@
     </row>
     <row r="39">
       <c r="B39">
-        <v>0.50871556304006582</v>
+        <v>0.41968552327866016</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -606,7 +696,7 @@
         <v>13</v>
       </c>
       <c r="B40">
-        <v>0.12883143677366876</v>
+        <v>0.099665637202006607</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -617,7 +707,7 @@
     </row>
     <row r="41">
       <c r="B41">
-        <v>0.038899999999999997</v>
+        <v>0.08683548218746473</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -628,7 +718,7 @@
     </row>
     <row r="42">
       <c r="B42">
-        <v>0.36153408907932943</v>
+        <v>0.80349888061052865</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -642,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="B43">
-        <v>0.14004682560972265</v>
+        <v>0.020325548397372672</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -653,7 +743,7 @@
     </row>
     <row r="44">
       <c r="B44">
-        <v>0.10244152317586383</v>
+        <v>0.13778407609772472</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -664,7 +754,7 @@
     </row>
     <row r="45">
       <c r="B45">
-        <v>0.74751165121441354</v>
+        <v>0.80445862906722865</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -678,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="B46">
-        <v>0.2836237198219313</v>
+        <v>0.10488490401437629</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -689,7 +779,7 @@
     </row>
     <row r="47">
       <c r="B47">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -700,7 +790,7 @@
     </row>
     <row r="48">
       <c r="B48">
-        <v>0.29509858100348535</v>
+        <v>0.39067500018321083</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -714,7 +804,7 @@
         <v>16</v>
       </c>
       <c r="B49">
-        <v>0.095351156470817683</v>
+        <v>0.25857005791003773</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -725,7 +815,7 @@
     </row>
     <row r="50">
       <c r="B50">
-        <v>0.12636596457952728</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -736,7 +826,7 @@
     </row>
     <row r="51">
       <c r="B51">
-        <v>0.76828287894965508</v>
+        <v>0.31313474125129276</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -750,35 +840,35 @@
         <v>17</v>
       </c>
       <c r="B52">
-        <v>0.10488490401437629</v>
+        <v>0.14620654336060132</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>1.1360228030968871</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="B53">
-        <v>0.038899999999999997</v>
+        <v>0.038913022582103343</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
-        <v>2.2732623201869417</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="B54">
-        <v>0.85609999999999997</v>
+        <v>0.50131047579329147</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>4.5528301227368324</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
@@ -786,7 +876,7 @@
         <v>18</v>
       </c>
       <c r="B55">
-        <v>0.044240679168123381</v>
+        <v>0.057625808971703489</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -797,7 +887,7 @@
     </row>
     <row r="56">
       <c r="B56">
-        <v>0.13670771006359447</v>
+        <v>0.23187311472200176</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -808,7 +898,7 @@
     </row>
     <row r="57">
       <c r="B57">
-        <v>0.56090523083011179</v>
+        <v>0.42054987481563899</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -833,24 +923,1104 @@
     </row>
     <row r="59">
       <c r="B59">
-        <v>0.038899999999999997</v>
+        <v>0.12454475549067914</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>2.2319532042837458</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
       <c r="B60">
-        <v>0.71097568878688522</v>
+        <v>0.70060014118092462</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>4.6697648852035627</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61">
+        <v>0.016407089703985512</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64">
+        <v>0.18712408629129851</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66">
+        <v>0.4634311757883573</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>4.775015131828944</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>4.9324049583496867</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70">
+        <v>0.16021356377024829</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71">
+        <v>0.11666582491436807</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72">
+        <v>0.71312061131538373</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>2.3136651563835766</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75">
+        <v>0.64010610120638178</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>4.6330250531179606</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78">
+        <v>0.32695495915992484</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B82">
+        <v>0.018597604919930788</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>2.1189239884970359</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84">
+        <v>0.70534402069676394</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>4.5027027747087196</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86">
+        <v>0.1972454907915121</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87">
+        <v>0.53407747475450362</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88">
+        <v>0.16455680607891224</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89">
+        <v>0.70966610045251466</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90">
+        <v>0.059418473272549045</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92">
+        <v>0.056318573375977996</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93">
+        <v>0.77835976871528056</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>4.8983421045372655</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B94">
+        <v>0.081035248012091554</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95">
+        <v>0.25753233256516078</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96">
+        <v>0.65143241942274765</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98">
+        <v>0.46698367165737575</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99">
+        <v>0.33940336554567158</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100">
+        <v>0.16455680607891224</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102">
+        <v>0.24164461855778407</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B103">
+        <v>0.16221405708895698</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104">
+        <v>0.19279237913754721</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105">
+        <v>0.45328837294023988</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B106">
+        <v>0.094506348292471634</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107">
+        <v>0.13410633402361008</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108">
+        <v>0.76138731768391832</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109">
+        <v>0.32005893034899957</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110">
+        <v>0.26394634960804281</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111">
+        <v>0.32695495915992484</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112">
+        <v>0.095101790225259025</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113">
+        <v>0.41013506656690923</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114">
+        <v>0.4847631432078317</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B115">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116">
+        <v>0.19892182574868211</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117">
+        <v>0.67696815215994177</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>4.320620409334909</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B118">
+        <v>0.05689326616893059</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119">
+        <v>0.10082299145213132</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120">
+        <v>0.57144431472306323</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B121">
+        <v>0.03702264012365164</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122">
+        <v>0.15492975176788737</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123">
+        <v>0.2746628411041192</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B124">
+        <v>0.071509740455303131</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125">
+        <v>0.31735353630318247</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126">
+        <v>0.52643992033621623</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B127">
+        <v>0.14620654336060132</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128">
+        <v>0.31735353630318247</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129">
+        <v>0.054239385126363837</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B130">
+        <v>0.24943875424365372</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132">
+        <v>0.32695495915992484</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>4.9964943985810839</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B133">
+        <v>0.016407089703985512</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134">
+        <v>0.33702103269435613</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>2.448134007035502</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135">
+        <v>0.40204549242122511</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>4.9283833180027621</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B136">
+        <v>0.0074802093413190301</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138">
+        <v>0.60067808489944663</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B139">
+        <v>0.16221405708895698</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140">
+        <v>0.1595023919922639</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141">
+        <v>0.32695495915992484</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B142">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144">
+        <v>0.38105176926118789</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>5.008698713486889</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B145">
+        <v>0.20724423354773802</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147">
+        <v>0.18508068132610495</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>4.9324049583496867</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B148">
+        <v>0.10488490401437629</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149">
+        <v>0.038913022582103343</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150">
+        <v>0.26633918007995455</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>